<commit_message>
Category and organic analysis with analytical data
</commit_message>
<xml_diff>
--- a/input/match_files/prod_match_2.xlsx
+++ b/input/match_files/prod_match_2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gsk-centrum\input\match_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gsk-centrum-classic\input\match_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A5FA6D-D7EB-4EAC-8CD8-4975A29B7AF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBDEC1B-AEF5-48B8-99DC-364598C330F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Sensory_name</t>
   </si>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t>Analytical_name</t>
+  </si>
+  <si>
+    <t>CVS Organic Multivitamin - (Product B - Yellow Gummy)</t>
+  </si>
+  <si>
+    <t>Spring Valley Adult Organic Multivitamin (Product A- Red Gummy)</t>
+  </si>
+  <si>
+    <t>CVS Health Organic Womens Multi</t>
+  </si>
+  <si>
+    <t>Spring Valley Womens Multi</t>
   </si>
 </sst>
 </file>
@@ -399,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +503,24 @@
         <v>9</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>